<commit_message>
Writing automation tests for checking file type
</commit_message>
<xml_diff>
--- a/TestyAPI_Zadanie-rekrutacyjne.xlsx
+++ b/TestyAPI_Zadanie-rekrutacyjne.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zadanie rekrutacyjne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD4E34D-BEC3-4A02-949C-E943DF22B85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8436E0-8B46-4255-910D-2EAC0B388050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ST1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t>Scenariusz testowy 1</t>
   </si>
@@ -124,7 +124,43 @@
     <t>3. W tym samym adresie po kluczu wpisać "&amp;file_type=json"</t>
   </si>
   <si>
-    <t>Dla podanego klucza interfejsu powinniśmy otrzymać listę danych ekonomicznych w formacie JSON oraz status HTTP 200</t>
+    <t>Uzyskiwanie danych ekonomicznych dla typu danych XML</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla dowolnego typu danych (innego niż JSON/XML)</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po kluczu wpisać "&amp;file_type=abcd"</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych gdy metoda HTTP jest inna niż GET</t>
+  </si>
+  <si>
+    <t>Przypadek testowy 5</t>
+  </si>
+  <si>
+    <t>2. Wybrać metodę "POST"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po kluczu wpisać "&amp;file_type=xml"</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla pustego typu danych</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po kluczu wpisać "&amp;file_type="</t>
+  </si>
+  <si>
+    <t>Dla podanego formatu danych powinniśmy otrzymać listę danych ekonomicznych w formacie JSON oraz status HTTP 200</t>
+  </si>
+  <si>
+    <t>Dla podanego formatu danych powinniśmy otrzymać listę danych ekonomicznych w formacie XML oraz status HTTP 200</t>
+  </si>
+  <si>
+    <t>Dla podanego formatu danych nie powinniśmy otrzymać listy danych ekonomicznych oraz powinniśmy otrzymać jeden ze statusów z grupy 4xx.</t>
+  </si>
+  <si>
+    <t>Dla podanego formatu danych powinniśmy otrzymać listę danych ekonomicznych oraz powinniśmy otrzymać status 200. Dane powinny być w formacie XML, ponieważ jest on domyślny, a format danych nie jest parametrem wymaganym, więc może pozostać pusty.</t>
   </si>
 </sst>
 </file>
@@ -410,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A999"/>
+  <dimension ref="A1:A997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -674,22 +710,70 @@
       </c>
     </row>
     <row r="64" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1607,8 +1691,6 @@
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1620,7 +1702,7 @@
   <dimension ref="A1:A954"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="Y52" sqref="Y52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1700,71 +1782,215 @@
     </row>
     <row r="18" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="25" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="32" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Writing automation tests for checking dates
</commit_message>
<xml_diff>
--- a/TestyAPI_Zadanie-rekrutacyjne.xlsx
+++ b/TestyAPI_Zadanie-rekrutacyjne.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zadanie rekrutacyjne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8436E0-8B46-4255-910D-2EAC0B388050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC51A49-30DD-48A0-A684-F0D025ED752C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ST1" sheetId="1" r:id="rId1"/>
     <sheet name="ST2" sheetId="2" r:id="rId2"/>
+    <sheet name="ST3" sheetId="3" r:id="rId3"/>
+    <sheet name="ST4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="71">
   <si>
     <t>Scenariusz testowy 1</t>
   </si>
@@ -161,6 +163,84 @@
   </si>
   <si>
     <t>Dla podanego formatu danych powinniśmy otrzymać listę danych ekonomicznych oraz powinniśmy otrzymać status 200. Dane powinny być w formacie XML, ponieważ jest on domyślny, a format danych nie jest parametrem wymaganym, więc może pozostać pusty.</t>
+  </si>
+  <si>
+    <t>Scenariusz testowy 3</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla podanych dat</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla danej daty od</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla danej daty do</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla prawidłowych dat od-do</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla nieprawidłowych dat od-do (data do jest wcześniejsza niż data od)</t>
+  </si>
+  <si>
+    <t>Dla podanej daty powinniśmy otrzymać listę tych danych ekonomicznych, których data od jest późniejsza lub taka sama jak podana w adresie url oraz status HTTP 200</t>
+  </si>
+  <si>
+    <t>Dla podanej daty powinniśmy otrzymać listę tych danych ekonomicznych, których data do jest wcześniejsza lub taka sama jak podana w adresie url oraz status HTTP 200</t>
+  </si>
+  <si>
+    <t>Dla podanych dat powinniśmy otrzymać listę tych danych ekonomicznych, których daty mieszczą się w przedziale dat wpiisanych w adresie url oraz status HTTP 200</t>
+  </si>
+  <si>
+    <t>Dla podanych dat nie powinniśmy otrzymać listy danych ekonomicznych, ponieważ zakres dat jest nieprawidłowy. Powinniśmy otrzymać jeden ze statusów z grupy 4xx.</t>
+  </si>
+  <si>
+    <t>Dla podanych dat nie powinniśmy otrzymać listy danych ekonomicznych, ponieważ format dat jest nieprawidłowy. Powinniśmy otrzymać jeden ze statusów z grupy 4xx.</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla określonego limitu danych</t>
+  </si>
+  <si>
+    <t>1. W adresie URL, po słowie "releases" umieścić dalszą część adresu "?api_key=" z prawidłowym kluczem interfejsu oraz po kluczu dodać "&amp;file_type=json"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;realtime_start=2024-05-01"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;realtime_end=2024-04-30"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;realtime_start=2024-04-01&amp;realtime_end=2024-05-10"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;realtime_start=2024-05-01&amp;realtime_end=2024-04-10"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;realtime_start=01-04-2024&amp;realtime_end=30-04-2024"</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla dat o nieprawidłowym formacie (daty od i do)</t>
+  </si>
+  <si>
+    <t>Przypadek testowy 6</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla dat o nieprawidłowym formacie (tylko data do)</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;realtime_end=30-04-2024"</t>
+  </si>
+  <si>
+    <t>Scenariusz testowy 4</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla limitu danych równego 10</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po kluczu wpisać "&amp;limit=10"</t>
+  </si>
+  <si>
+    <t>Dla podanego limitu danych powinniśmy otrzymać listę pierwszych 10ciu danych z listy oraz status HTTP 200</t>
   </si>
 </sst>
 </file>
@@ -449,7 +529,7 @@
   <dimension ref="A1:A997"/>
   <sheetViews>
     <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="K82" sqref="K82"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1701,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F86B0AA-E9BB-462E-A326-3A4E7CC96E0C}">
   <dimension ref="A1:A954"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y52" sqref="Y52"/>
     </sheetView>
   </sheetViews>
@@ -2869,4 +2949,2400 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7CEEBD-6AE4-4906-9813-95D1ADD06221}">
+  <dimension ref="A1:A954"/>
+  <sheetViews>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="L82" sqref="L82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="26" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B5C9DE-5057-4155-A6C9-8B17981CEC3B}">
+  <dimension ref="A1:A954"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="26" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+    </row>
+    <row r="56" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+    </row>
+    <row r="59" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+    </row>
+    <row r="66" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+    </row>
+    <row r="72" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+    </row>
+    <row r="75" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+    </row>
+    <row r="82" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+    </row>
+    <row r="83" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Writing automation tests for checkking paging parameters
</commit_message>
<xml_diff>
--- a/TestyAPI_Zadanie-rekrutacyjne.xlsx
+++ b/TestyAPI_Zadanie-rekrutacyjne.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zadanie rekrutacyjne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC51A49-30DD-48A0-A684-F0D025ED752C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B55AE2-43A3-4769-8F31-B3ED38D245B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="108">
   <si>
     <t>Scenariusz testowy 1</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Dla podanych dat nie powinniśmy otrzymać listy danych ekonomicznych, ponieważ format dat jest nieprawidłowy. Powinniśmy otrzymać jeden ze statusów z grupy 4xx.</t>
   </si>
   <si>
-    <t>Uzyskiwanie danych ekonomicznych dla określonego limitu danych</t>
-  </si>
-  <si>
     <t>1. W adresie URL, po słowie "releases" umieścić dalszą część adresu "?api_key=" z prawidłowym kluczem interfejsu oraz po kluczu dodać "&amp;file_type=json"</t>
   </si>
   <si>
@@ -234,13 +231,127 @@
     <t>Scenariusz testowy 4</t>
   </si>
   <si>
-    <t>Uzyskiwanie danych ekonomicznych dla limitu danych równego 10</t>
-  </si>
-  <si>
-    <t>3. W tym samym adresie po kluczu wpisać "&amp;limit=10"</t>
-  </si>
-  <si>
-    <t>Dla podanego limitu danych powinniśmy otrzymać listę pierwszych 10ciu danych z listy oraz status HTTP 200</t>
+    <t>Uzyskiwanie danych ekonomicznych dla określonego stronnicowania</t>
+  </si>
+  <si>
+    <t>Dla podanego limitu danych nie powinniśmy otrzymać listy danych ekonomicznych, ponieważ wartość limitu jest poza przyjętym zakresem. Powinniśmy otrzymać jeden ze statusów z grupy 4xx.</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla limitu danych równego 1, 10 i 1000</t>
+  </si>
+  <si>
+    <t>Dla podanych limitów danych powinniśmy otrzymać listę najpierw z jednym obiektem, potem listę pierwszych 10ciu obiektów, a na koniec listę pierwszych 1000 obiektów (lub wszystkich obiektów jeśli jest ich mniej niż 10 lub 1000). Powinniśmy także otrzymać status HTTP 200.</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla limitu danych równego 0 oraz 1001</t>
+  </si>
+  <si>
+    <t>7. Wysłać request</t>
+  </si>
+  <si>
+    <t>8. Zweryfikować dane</t>
+  </si>
+  <si>
+    <t>10. Wysłać request</t>
+  </si>
+  <si>
+    <t>11. Zweryfikować dane</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla offsetu równego -1</t>
+  </si>
+  <si>
+    <t>Dla podanego offsetu nie powinniśmy otrzymać listy z danymi, ponieważ wartość tego parametru wykracza poza przyjęty zakres. Powinniśmy także otrzymać jeden ze statusów z grupy 4xx.</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie posortowanych danych ekonomicznych - release_id</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;limit=1"</t>
+  </si>
+  <si>
+    <t>6. W tym samym adresie po typie danych wpisać "&amp;limit=10"</t>
+  </si>
+  <si>
+    <t>9. W tym samym adresie po typie danych wpisać "&amp;limit=1000"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;limit=0"</t>
+  </si>
+  <si>
+    <t>6. W tym samym adresie po typie danych wpisać "&amp;limit=1001"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;offset=2"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;offset=-1"</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;order_by=release_id&amp;sort_order=asc"</t>
+  </si>
+  <si>
+    <t>6. W adresie URL zmienić parametr "sort_order=desc"</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie posortowanych danych ekonomicznych - name</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;order_by=name&amp;sort_order=asc"</t>
+  </si>
+  <si>
+    <t>Dla podanego sortowania powinniśmy otrzymać listę z danymi posortowaną najpierw rosnąco, a potem malejąco po release_id. Powinniśmy także otrzymać status HTTP 200.</t>
+  </si>
+  <si>
+    <t>Dla podanego sortowania powinniśmy otrzymać listę z danymi posortowaną najpierw rosnąco, a potem malejąco po name. Powinniśmy także otrzymać status HTTP 200.</t>
+  </si>
+  <si>
+    <t>Przypadek testowy 7</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie posortowanych danych ekonomicznych - press_release</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;order_by=press_release&amp;sort_order=asc"</t>
+  </si>
+  <si>
+    <t>Dla podanego sortowania powinniśmy otrzymać listę z danymi posortowaną najpierw rosnąco, a potem malejąco po press_release. Powinniśmy także otrzymać status HTTP 200.</t>
+  </si>
+  <si>
+    <t>Przypadek testowy 8</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;order_by=realtime_start&amp;sort_order=asc"</t>
+  </si>
+  <si>
+    <t>Dla podanego sortowania powinniśmy otrzymać listę z danymi posortowaną najpierw rosnąco, a potem malejąco po realtime_start. Powinniśmy także otrzymać status HTTP 200.</t>
+  </si>
+  <si>
+    <t>Przypadek testowy 9</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie posortowanych danych ekonomicznych - realtime_start</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie posortowanych danych ekonomicznych - realtime_end</t>
+  </si>
+  <si>
+    <t>3. W tym samym adresie po typie danych wpisać "&amp;order_by=realtime_end&amp;sort_order=asc"</t>
+  </si>
+  <si>
+    <t>Dla podanego sortowania powinniśmy otrzymać listę z danymi posortowaną najpierw rosnąco, a potem malejąco po realtime_end. Powinniśmy także otrzymać status HTTP 200.</t>
+  </si>
+  <si>
+    <t>6. W tym samym adresie po typie danych wpisać "&amp;offset=0"</t>
+  </si>
+  <si>
+    <t>Dla podanych offsetów powinniśmy otrzymać najpierw listę z danymi, pomijając 2 pierwsze obkiety, a potem listę ze wszystkimi obiektami, a na koniec listę z zerową liczbą obiektów. Powinniśmy także otrzymać status HTTP 200.</t>
+  </si>
+  <si>
+    <t>Uzyskiwanie danych ekonomicznych dla offsetu równego 2, 0 oraz liczby większej lub równej ilości danych</t>
+  </si>
+  <si>
+    <t>6. W tym samym adresie po typie danych zmienić offset na wartość większą lub równą ilości danych</t>
   </si>
 </sst>
 </file>
@@ -304,13 +415,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -528,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A997"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
+    <sheetView topLeftCell="A50" workbookViewId="0">
       <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
@@ -2955,8 +3067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7CEEBD-6AE4-4906-9813-95D1ADD06221}">
   <dimension ref="A1:A954"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="L82" sqref="L82"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3005,7 +3117,7 @@
     </row>
     <row r="11" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3015,7 +3127,7 @@
     </row>
     <row r="13" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3069,7 +3181,7 @@
     </row>
     <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3079,7 +3191,7 @@
     </row>
     <row r="29" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3133,7 +3245,7 @@
     </row>
     <row r="43" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3143,7 +3255,7 @@
     </row>
     <row r="45" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3197,7 +3309,7 @@
     </row>
     <row r="59" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3207,7 +3319,7 @@
     </row>
     <row r="61" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3239,7 +3351,7 @@
     </row>
     <row r="69" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3261,7 +3373,7 @@
     </row>
     <row r="75" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3271,7 +3383,7 @@
     </row>
     <row r="77" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3298,12 +3410,12 @@
     <row r="83" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="84" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3325,7 +3437,7 @@
     </row>
     <row r="91" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3335,7 +3447,7 @@
     </row>
     <row r="93" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4223,10 +4335,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B5C9DE-5057-4155-A6C9-8B17981CEC3B}">
-  <dimension ref="A1:A954"/>
+  <dimension ref="A1:A972"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4237,12 +4349,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4253,7 +4365,7 @@
     </row>
     <row r="5" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4275,7 +4387,7 @@
     </row>
     <row r="11" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4285,7 +4397,7 @@
     </row>
     <row r="13" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4298,271 +4410,679 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>12</v>
+      <c r="A17" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="20" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="21" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="25" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="A26" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-    </row>
+      <c r="A27" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-    </row>
-    <row r="31" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-    </row>
-    <row r="32" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A30" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+      <c r="A33" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-    </row>
-    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A34" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A37" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
+      <c r="A39" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="40" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+      <c r="A40" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="41" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+      <c r="A42" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="43" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-    </row>
-    <row r="44" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-    </row>
+      <c r="A43" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
+      <c r="A45" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="46" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-    </row>
-    <row r="47" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-    </row>
-    <row r="48" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A46" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="49" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-    </row>
-    <row r="50" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-    </row>
-    <row r="51" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A49" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="52" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
+      <c r="A52" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="53" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-    </row>
-    <row r="54" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A53" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="55" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
+      <c r="A55" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="56" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-    </row>
-    <row r="57" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A56" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="58" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
+      <c r="A58" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="59" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
+      <c r="A59" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="60" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
+      <c r="A60" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="61" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
+      <c r="A61" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="62" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-    </row>
-    <row r="63" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-    </row>
-    <row r="64" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A62" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="65" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-    </row>
-    <row r="66" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-    </row>
-    <row r="67" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A65" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="68" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-    </row>
-    <row r="69" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-    </row>
-    <row r="70" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A68" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="71" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-    </row>
-    <row r="72" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-    </row>
-    <row r="73" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A71" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="74" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
+      <c r="A74" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="75" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
+      <c r="A75" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="76" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
+      <c r="A76" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="77" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
+      <c r="A77" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="78" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-    </row>
-    <row r="79" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-    </row>
-    <row r="80" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A78" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="81" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-    </row>
-    <row r="82" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-    </row>
-    <row r="83" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A81" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="85" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="88" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5341,6 +5861,24 @@
     <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Small updates in automation tests
</commit_message>
<xml_diff>
--- a/TestyAPI_Zadanie-rekrutacyjne.xlsx
+++ b/TestyAPI_Zadanie-rekrutacyjne.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zadanie rekrutacyjne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B55AE2-43A3-4769-8F31-B3ED38D245B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1738D3-2185-4D61-91D3-A9A5DA02DD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,14 +415,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1893,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F86B0AA-E9BB-462E-A326-3A4E7CC96E0C}">
   <dimension ref="A1:A954"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="Y52" sqref="Y52"/>
     </sheetView>
   </sheetViews>
@@ -3067,7 +3066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7CEEBD-6AE4-4906-9813-95D1ADD06221}">
   <dimension ref="A1:A954"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
@@ -4337,8 +4336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B5C9DE-5057-4155-A6C9-8B17981CEC3B}">
   <dimension ref="A1:A972"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4742,7 +4741,7 @@
       </c>
     </row>
     <row r="95" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
+      <c r="A95" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4821,7 +4820,7 @@
       </c>
     </row>
     <row r="114" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="6" t="s">
+      <c r="A114" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4900,7 +4899,7 @@
       </c>
     </row>
     <row r="133" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="6" t="s">
+      <c r="A133" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4979,7 +4978,7 @@
       </c>
     </row>
     <row r="152" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="6" t="s">
+      <c r="A152" t="s">
         <v>87</v>
       </c>
     </row>
@@ -5058,7 +5057,7 @@
       </c>
     </row>
     <row r="171" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="6" t="s">
+      <c r="A171" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>